<commit_message>
New change to excel
</commit_message>
<xml_diff>
--- a/public/projects.xlsx
+++ b/public/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new portfolio\rohan-learns-ai-main\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BA4DA-C06C-42F4-AC8B-0477CF06839D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783DB7D-EDEB-4B86-8FF0-BAE8F4692272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0AB1B34F-2472-4F04-A4F2-B478495E2144}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>Blur Buddy</t>
-  </si>
-  <si>
     <t>A program that would work as a virtual camera and censor specific subject/object</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>https://github.com/JokhonApniRohan/Censor-Buddy</t>
+  </si>
+  <si>
+    <t>Censor Buddy</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,16 +708,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>

</xml_diff>